<commit_message>
Morning of April 13
</commit_message>
<xml_diff>
--- a/TestTrack_Since0403.xlsx
+++ b/TestTrack_Since0403.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="12045" windowHeight="4680"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="12045" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Transformers" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="112">
   <si>
     <t>P2B-PRI-02</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -394,6 +394,14 @@
   </si>
   <si>
     <t>Corner3-loop4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corner4-loop4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1058,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1084,15 +1092,19 @@
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.25" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A1" s="2">
         <f ca="1">NOW()</f>
-        <v>42103.892339120372</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+        <v>42107.391311111111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,8 +1159,20 @@
       <c r="R2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S2" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1191,8 +1215,20 @@
       <c r="R3" s="39">
         <v>42103.397222222222</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S3" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="U3" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="39">
+        <v>42104.397222222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
@@ -1224,8 +1260,14 @@
       <c r="P4" s="42"/>
       <c r="Q4" s="43"/>
       <c r="R4" s="47"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="42"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="47"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1259,8 +1301,14 @@
       <c r="P5" s="44"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="48"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="44"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="48"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
@@ -1313,8 +1361,20 @@
       <c r="R6" s="39">
         <v>42103.397222222222</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S6" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="U6" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="V6" s="39">
+        <v>42104.397222222222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -1366,8 +1426,20 @@
       <c r="R7" s="18">
         <v>42103.397222222222</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S7" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="V7" s="18">
+        <v>42104.397222222222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
@@ -1419,8 +1491,20 @@
       <c r="R8" s="24">
         <v>42103.397222222222</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S8" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="U8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="V8" s="24">
+        <v>42104.397222222222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>10</v>
       </c>
@@ -1469,8 +1553,20 @@
       <c r="R9" s="46">
         <v>42103.397222222222</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T9" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="U9" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="V9" s="46">
+        <v>42104.397222222222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
@@ -1519,8 +1615,20 @@
       <c r="R10" s="15">
         <v>42103.397222222222</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S10" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" s="15">
+        <v>42104.397222222222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>59</v>
       </c>
@@ -1537,8 +1645,14 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="28"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="28"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>60</v>
       </c>
@@ -1554,6 +1668,12 @@
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="34"/>
+      <c r="S12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1585,7 +1705,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="2">
         <f ca="1">NOW()</f>
-        <v>42103.892339120372</v>
+        <v>42107.391311111111</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
test status before the National Labour Day!
</commit_message>
<xml_diff>
--- a/TestTrack_Since0403.xlsx
+++ b/TestTrack_Since0403.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="735" windowWidth="2130" windowHeight="4200" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="795" windowWidth="2130" windowHeight="4140"/>
   </bookViews>
   <sheets>
     <sheet name="Transformers" sheetId="1" r:id="rId1"/>
@@ -1400,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1433,7 +1433,7 @@
     <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="B1" s="2">
         <f ca="1">NOW()</f>
-        <v>42121.473885416664</v>
+        <v>42122.790069328701</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
@@ -2064,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2084,7 +2084,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="2">
         <f ca="1">NOW()</f>
-        <v>42121.473885416664</v>
+        <v>42122.790069328701</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>